<commit_message>
Update issue 206 EFLIB:   Add lock function to atomic.   Add fixed_string::mutable_raw_string().   Remove compiler_infos from sasl/enums.   Start to split function definition from function type.     1. Rename function_type to function_full_def, parameter to parameter_full.     2. Add function_type, function_def and parameter.   Porting name mangling to pety, but not been used yet.
</commit_message>
<xml_diff>
--- a/doc/contents/materials/Performance.xlsx
+++ b/doc/contents/materials/Performance.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="20120705" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="20121215D" sheetId="2" r:id="rId2"/>
+    <sheet name="20121215R" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Boost::Unordered_Map</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -65,22 +65,40 @@
     <t>Perf (Total)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>Optimized type classifications</t>
+  </si>
+  <si>
+    <t>Optimized type id</t>
+  </si>
+  <si>
+    <t>read-only string optimization</t>
+  </si>
+  <si>
+    <t>mangling optimization</t>
+  </si>
+  <si>
+    <t>Read only string in parser and symbol</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -112,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -120,11 +138,44 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -154,6 +205,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -165,7 +284,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -200,7 +319,7 @@
             <c:numRef>
               <c:f>'20120705'!$B$2:$B$11</c:f>
               <c:numCache>
-                <c:formatCode>G/通用格式</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>4967</c:v>
@@ -255,7 +374,7 @@
             <c:numRef>
               <c:f>'20120705'!$C$2:$C$11</c:f>
               <c:numCache>
-                <c:formatCode>G/通用格式</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>4910</c:v>
@@ -310,7 +429,7 @@
             <c:numRef>
               <c:f>'20120705'!$D$2:$D$11</c:f>
               <c:numCache>
-                <c:formatCode>G/通用格式</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>4764</c:v>
@@ -365,7 +484,7 @@
             <c:numRef>
               <c:f>'20120705'!$E$2:$E$11</c:f>
               <c:numCache>
-                <c:formatCode>G/通用格式</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>4759</c:v>
@@ -420,7 +539,7 @@
             <c:numRef>
               <c:f>'20120705'!$F$2:$F$11</c:f>
               <c:numCache>
-                <c:formatCode>G/通用格式</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>4703</c:v>
@@ -475,7 +594,7 @@
             <c:numRef>
               <c:f>'20120705'!$G$2:$G$11</c:f>
               <c:numCache>
-                <c:formatCode>G/通用格式</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>4503</c:v>
@@ -522,11 +641,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="92812800"/>
-        <c:axId val="180620672"/>
+        <c:axId val="98310144"/>
+        <c:axId val="83859072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92812800"/>
+        <c:axId val="98310144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -535,7 +654,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="180620672"/>
+        <c:crossAx val="83859072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -543,25 +662,24 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="180620672"/>
+        <c:axId val="83859072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="G/通用格式" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92812800"/>
+        <c:crossAx val="98310144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -619,7 +737,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="E0E0E0"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -900,22 +1018,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="60">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -938,7 +1056,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -961,7 +1079,7 @@
         <v>4503</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -984,7 +1102,7 @@
         <v>4522</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1007,7 +1125,7 @@
         <v>4409</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1030,7 +1148,7 @@
         <v>4470</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1053,7 +1171,7 @@
         <v>4483</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1076,7 +1194,7 @@
         <v>4475</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1099,7 +1217,7 @@
         <v>4505</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1122,7 +1240,7 @@
         <v>4518</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1145,7 +1263,7 @@
         <v>4501</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1168,65 +1286,65 @@
         <v>4517</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="1">
-        <f>AVERAGE(B2:B11)</f>
+        <f t="shared" ref="B12:G12" si="0">AVERAGE(B2:B11)</f>
         <v>4984.6000000000004</v>
       </c>
       <c r="C12" s="1">
-        <f>AVERAGE(C2:C11)</f>
+        <f t="shared" si="0"/>
         <v>4880.8</v>
       </c>
       <c r="D12" s="1">
-        <f>AVERAGE(D2:D11)</f>
+        <f t="shared" si="0"/>
         <v>4707.8</v>
       </c>
       <c r="E12" s="1">
-        <f>AVERAGE(E2:E11)</f>
+        <f t="shared" si="0"/>
         <v>4739</v>
       </c>
       <c r="F12" s="1">
-        <f>AVERAGE(F2:F11)</f>
+        <f t="shared" si="0"/>
         <v>4672</v>
       </c>
       <c r="G12" s="1">
-        <f>AVERAGE(G2:G11)</f>
+        <f t="shared" si="0"/>
         <v>4490.3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="1">
-        <f>_xlfn.VAR.S(B2:B11)</f>
+        <f t="shared" ref="B13:G13" si="1">_xlfn.VAR.S(B2:B11)</f>
         <v>1471.1555555555558</v>
       </c>
       <c r="C13" s="1">
-        <f>_xlfn.VAR.S(C2:C11)</f>
+        <f t="shared" si="1"/>
         <v>1567.0666666666668</v>
       </c>
       <c r="D13" s="1">
-        <f>_xlfn.VAR.S(D2:D11)</f>
+        <f t="shared" si="1"/>
         <v>4277.7333333333336</v>
       </c>
       <c r="E13" s="1">
-        <f>_xlfn.VAR.S(E2:E11)</f>
+        <f t="shared" si="1"/>
         <v>1057.1111111111111</v>
       </c>
       <c r="F13" s="1">
-        <f>_xlfn.VAR.S(F2:F11)</f>
+        <f t="shared" si="1"/>
         <v>2762.8888888888887</v>
       </c>
       <c r="G13" s="1">
-        <f>_xlfn.VAR.S(G2:G11)</f>
+        <f t="shared" si="1"/>
         <v>1142.9000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -1254,7 +1372,7 @@
         <v>0.999999877202561</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -1283,7 +1401,7 @@
       </c>
       <c r="H15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -1311,7 +1429,7 @@
         <v>1.1100817317328464</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
@@ -1321,7 +1439,7 @@
       <c r="G17"/>
       <c r="H17"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
@@ -1331,7 +1449,7 @@
       <c r="G18"/>
       <c r="H18"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
@@ -1341,7 +1459,7 @@
       <c r="G19"/>
       <c r="H19"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
@@ -1351,7 +1469,7 @@
       <c r="G20"/>
       <c r="H20"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
@@ -1361,7 +1479,7 @@
       <c r="G21"/>
       <c r="H21"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -1371,7 +1489,7 @@
       <c r="G22"/>
       <c r="H22"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -1381,7 +1499,7 @@
       <c r="G23"/>
       <c r="H23"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -1391,7 +1509,7 @@
       <c r="G24"/>
       <c r="H24"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -1401,7 +1519,7 @@
       <c r="G25"/>
       <c r="H25"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
@@ -1410,7 +1528,7 @@
       <c r="G26"/>
       <c r="H26"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
@@ -1419,7 +1537,7 @@
       <c r="G27"/>
       <c r="H27"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
@@ -1428,13 +1546,13 @@
       <c r="G28"/>
       <c r="H28"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30"/>
@@ -1444,13 +1562,13 @@
   <dataConsolidate/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B15:G16">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1462,14 +1580,354 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="69" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>5610</v>
+      </c>
+      <c r="C2" s="4">
+        <v>5406</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>5512</v>
+      </c>
+      <c r="C3" s="4">
+        <v>5702</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>5565</v>
+      </c>
+      <c r="C4" s="4">
+        <v>5414</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>5521</v>
+      </c>
+      <c r="C5" s="4">
+        <v>5421</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>5533</v>
+      </c>
+      <c r="C6" s="4">
+        <v>5412</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>5550</v>
+      </c>
+      <c r="C7" s="4">
+        <v>5388</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>5562</v>
+      </c>
+      <c r="C8" s="4">
+        <v>5393</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>5508</v>
+      </c>
+      <c r="C9" s="4">
+        <v>5369</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <v>5519</v>
+      </c>
+      <c r="C10" s="4">
+        <v>5389</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
+        <v>5539</v>
+      </c>
+      <c r="C11" s="4">
+        <v>5402</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="4">
+        <f>AVERAGE(B2:B11)</f>
+        <v>5541.9</v>
+      </c>
+      <c r="C12" s="4">
+        <f t="shared" ref="C12:G12" si="0">AVERAGE(C2:C11)</f>
+        <v>5429.6</v>
+      </c>
+      <c r="D12" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E12" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F12" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G12" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="4">
+        <f>_xlfn.VAR.S(B2:B11)</f>
+        <v>970.32222222222242</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" ref="C13:G13" si="1">_xlfn.VAR.S(C2:C11)</f>
+        <v>9393.1555555555569</v>
+      </c>
+      <c r="D13" s="4" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E13" s="4" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F13" s="4" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G13" s="4" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4">
+        <f>1-_xlfn.T.TEST(B2:B11,C2:C11,2,3)</f>
+        <v>0.9948174605524347</v>
+      </c>
+      <c r="D14" s="4" t="e">
+        <f>1-_xlfn.T.TEST(C2:C11,D2:D11,2,3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E14" s="4" t="e">
+        <f>1-_xlfn.T.TEST(D2:D11,E2:E11,2,3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F14" s="4" t="e">
+        <f>1-_xlfn.T.TEST(D2:D11,F2:F11,2,3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G14" s="4" t="e">
+        <f>1-_xlfn.T.TEST(F2:F11,G2:G11,2,3)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4">
+        <f>B12/C12</f>
+        <v>1.0206829232355974</v>
+      </c>
+      <c r="D15" s="4" t="e">
+        <f>C12/D12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E15" s="4" t="e">
+        <f>D12/E12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F15" s="4" t="e">
+        <f>D12/F12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G15" s="4" t="e">
+        <f>F12/G12</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4">
+        <f>B12/C12</f>
+        <v>1.0206829232355974</v>
+      </c>
+      <c r="D16" s="4" t="e">
+        <f>B12/D12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E16" s="4" t="e">
+        <f>B12/E12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F16" s="4" t="e">
+        <f>B12/F12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G16" s="4" t="e">
+        <f>B12/G12</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="B15:G16">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1477,9 +1935,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update issue 206 SASL:   Add function_type, function_def and parameter to visitor.   Update performance document.
</commit_message>
<xml_diff>
--- a/doc/contents/materials/Performance.xlsx
+++ b/doc/contents/materials/Performance.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Boost::Unordered_Map</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -69,19 +69,10 @@
     <t>Original</t>
   </si>
   <si>
-    <t>Optimized type classifications</t>
+    <t>Read only string in parser and symbol</t>
   </si>
   <si>
-    <t>Optimized type id</t>
-  </si>
-  <si>
-    <t>read-only string optimization</t>
-  </si>
-  <si>
-    <t>mangling optimization</t>
-  </si>
-  <si>
-    <t>Read only string in parser and symbol</t>
+    <t>Remove unused symbol insertion when parameter is anonymous</t>
   </si>
 </sst>
 </file>
@@ -641,11 +632,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="98310144"/>
-        <c:axId val="83859072"/>
+        <c:axId val="68269568"/>
+        <c:axId val="73832064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98310144"/>
+        <c:axId val="68269568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -654,7 +645,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83859072"/>
+        <c:crossAx val="73832064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -662,7 +653,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83859072"/>
+        <c:axId val="73832064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -673,7 +664,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98310144"/>
+        <c:crossAx val="68269568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1583,7 +1574,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1606,20 +1597,14 @@
         <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="4">
@@ -1631,7 +1616,9 @@
       <c r="C2" s="4">
         <v>5406</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="4">
+        <v>4765</v>
+      </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1646,7 +1633,9 @@
       <c r="C3" s="4">
         <v>5702</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4">
+        <v>4747</v>
+      </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -1661,7 +1650,9 @@
       <c r="C4" s="4">
         <v>5414</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="4">
+        <v>4771</v>
+      </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -1676,7 +1667,9 @@
       <c r="C5" s="4">
         <v>5421</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4">
+        <v>4754</v>
+      </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -1691,7 +1684,9 @@
       <c r="C6" s="4">
         <v>5412</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="4">
+        <v>4751</v>
+      </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -1706,7 +1701,9 @@
       <c r="C7" s="4">
         <v>5388</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="4">
+        <v>4812</v>
+      </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -1721,7 +1718,9 @@
       <c r="C8" s="4">
         <v>5393</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="4">
+        <v>4771</v>
+      </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -1736,7 +1735,9 @@
       <c r="C9" s="4">
         <v>5369</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4">
+        <v>4795</v>
+      </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -1751,7 +1752,9 @@
       <c r="C10" s="4">
         <v>5389</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="4">
+        <v>4736</v>
+      </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -1766,7 +1769,9 @@
       <c r="C11" s="4">
         <v>5402</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="4">
+        <v>4780</v>
+      </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -1783,9 +1788,9 @@
         <f t="shared" ref="C12:G12" si="0">AVERAGE(C2:C11)</f>
         <v>5429.6</v>
       </c>
-      <c r="D12" s="4" t="e">
+      <c r="D12" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>4768.2</v>
       </c>
       <c r="E12" s="4" t="e">
         <f t="shared" si="0"/>
@@ -1812,9 +1817,9 @@
         <f t="shared" ref="C13:G13" si="1">_xlfn.VAR.S(C2:C11)</f>
         <v>9393.1555555555569</v>
       </c>
-      <c r="D13" s="4" t="e">
+      <c r="D13" s="4">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>531.73333333333335</v>
       </c>
       <c r="E13" s="4" t="e">
         <f t="shared" si="1"/>
@@ -1840,9 +1845,9 @@
         <f>1-_xlfn.T.TEST(B2:B11,C2:C11,2,3)</f>
         <v>0.9948174605524347</v>
       </c>
-      <c r="D14" s="4" t="e">
+      <c r="D14" s="4">
         <f>1-_xlfn.T.TEST(C2:C11,D2:D11,2,3)</f>
-        <v>#DIV/0!</v>
+        <v>0.99999999869544887</v>
       </c>
       <c r="E14" s="4" t="e">
         <f>1-_xlfn.T.TEST(D2:D11,E2:E11,2,3)</f>
@@ -1868,9 +1873,9 @@
         <f>B12/C12</f>
         <v>1.0206829232355974</v>
       </c>
-      <c r="D15" s="4" t="e">
+      <c r="D15" s="4">
         <f>C12/D12</f>
-        <v>#DIV/0!</v>
+        <v>1.1387106245543392</v>
       </c>
       <c r="E15" s="4" t="e">
         <f>D12/E12</f>
@@ -1896,9 +1901,9 @@
         <f>B12/C12</f>
         <v>1.0206829232355974</v>
       </c>
-      <c r="D16" s="4" t="e">
+      <c r="D16" s="4">
         <f>B12/D12</f>
-        <v>#DIV/0!</v>
+        <v>1.1622624889895559</v>
       </c>
       <c r="E16" s="4" t="e">
         <f>B12/E12</f>

</xml_diff>

<commit_message>
Update issue 206 SASL:   Remove unused 'external' flag for intrinsic.   Add symbol::get_overload_position and symbol::unchecked_insert_overload        to optimize builtin function symbol registration.   Implements new built in function registration but not used and tested.
</commit_message>
<xml_diff>
--- a/doc/contents/materials/Performance.xlsx
+++ b/doc/contents/materials/Performance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="20120705" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
     <t>Boost::Unordered_Map</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -67,12 +67,6 @@
   </si>
   <si>
     <t>Original</t>
-  </si>
-  <si>
-    <t>Read only string in parser and symbol</t>
-  </si>
-  <si>
-    <t>Remove unused symbol insertion when parameter is anonymous</t>
   </si>
 </sst>
 </file>
@@ -139,7 +133,88 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -632,11 +707,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="68269568"/>
-        <c:axId val="73832064"/>
+        <c:axId val="87004672"/>
+        <c:axId val="71669376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="68269568"/>
+        <c:axId val="87004672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -645,7 +720,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73832064"/>
+        <c:crossAx val="71669376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -653,7 +728,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73832064"/>
+        <c:axId val="71669376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -664,7 +739,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68269568"/>
+        <c:crossAx val="87004672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1553,13 +1628,13 @@
   <dataConsolidate/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B15:G16">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1573,8 +1648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection sqref="A1:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1589,21 +1664,25 @@
     <col min="8" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="69" customHeight="1">
+    <row r="1" spans="1:7" ht="30" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="C1" s="2">
+        <v>1205</v>
+      </c>
+      <c r="D1" s="2">
+        <v>1209</v>
+      </c>
+      <c r="E1" s="2">
+        <v>1210</v>
+      </c>
+      <c r="F1" s="2">
+        <v>1211</v>
+      </c>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7">
@@ -1619,8 +1698,12 @@
       <c r="D2" s="4">
         <v>4765</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="E2" s="4">
+        <v>4811</v>
+      </c>
+      <c r="F2" s="4">
+        <v>4321</v>
+      </c>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7">
@@ -1636,8 +1719,12 @@
       <c r="D3" s="4">
         <v>4747</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="E3" s="4">
+        <v>4789</v>
+      </c>
+      <c r="F3" s="4">
+        <v>4334</v>
+      </c>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7">
@@ -1653,8 +1740,12 @@
       <c r="D4" s="4">
         <v>4771</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="E4" s="4">
+        <v>4796</v>
+      </c>
+      <c r="F4" s="4">
+        <v>4326</v>
+      </c>
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7">
@@ -1670,8 +1761,12 @@
       <c r="D5" s="4">
         <v>4754</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="E5" s="4">
+        <v>4769</v>
+      </c>
+      <c r="F5" s="4">
+        <v>4306</v>
+      </c>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7">
@@ -1687,8 +1782,12 @@
       <c r="D6" s="4">
         <v>4751</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="E6" s="4">
+        <v>4775</v>
+      </c>
+      <c r="F6" s="4">
+        <v>4295</v>
+      </c>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7">
@@ -1704,8 +1803,12 @@
       <c r="D7" s="4">
         <v>4812</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="E7" s="4">
+        <v>4778</v>
+      </c>
+      <c r="F7" s="4">
+        <v>4321</v>
+      </c>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7">
@@ -1721,8 +1824,12 @@
       <c r="D8" s="4">
         <v>4771</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="E8" s="4">
+        <v>4775</v>
+      </c>
+      <c r="F8" s="4">
+        <v>4314</v>
+      </c>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7">
@@ -1738,8 +1845,12 @@
       <c r="D9" s="4">
         <v>4795</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="E9" s="4">
+        <v>4792</v>
+      </c>
+      <c r="F9" s="4">
+        <v>4297</v>
+      </c>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7">
@@ -1755,8 +1866,12 @@
       <c r="D10" s="4">
         <v>4736</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="E10" s="4">
+        <v>4797</v>
+      </c>
+      <c r="F10" s="4">
+        <v>4296</v>
+      </c>
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7">
@@ -1772,8 +1887,12 @@
       <c r="D11" s="4">
         <v>4780</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="E11" s="4">
+        <v>4797</v>
+      </c>
+      <c r="F11" s="4">
+        <v>4295</v>
+      </c>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7">
@@ -1792,13 +1911,13 @@
         <f t="shared" si="0"/>
         <v>4768.2</v>
       </c>
-      <c r="E12" s="4" t="e">
+      <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F12" s="4" t="e">
+        <v>4787.8999999999996</v>
+      </c>
+      <c r="F12" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>4310.5</v>
       </c>
       <c r="G12" s="4" t="e">
         <f t="shared" si="0"/>
@@ -1821,13 +1940,13 @@
         <f t="shared" si="1"/>
         <v>531.73333333333335</v>
       </c>
-      <c r="E13" s="4" t="e">
+      <c r="E13" s="4">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F13" s="4" t="e">
+        <v>174.54444444444439</v>
+      </c>
+      <c r="F13" s="4">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>213.16666666666666</v>
       </c>
       <c r="G13" s="4" t="e">
         <f t="shared" si="1"/>
@@ -1849,13 +1968,13 @@
         <f>1-_xlfn.T.TEST(C2:C11,D2:D11,2,3)</f>
         <v>0.99999999869544887</v>
       </c>
-      <c r="E14" s="4" t="e">
+      <c r="E14" s="4">
         <f>1-_xlfn.T.TEST(D2:D11,E2:E11,2,3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F14" s="4" t="e">
+        <v>0.96603523046161688</v>
+      </c>
+      <c r="F14" s="4">
         <f>1-_xlfn.T.TEST(D2:D11,F2:F11,2,3)</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G14" s="4" t="e">
         <f>1-_xlfn.T.TEST(F2:F11,G2:G11,2,3)</f>
@@ -1877,13 +1996,13 @@
         <f>C12/D12</f>
         <v>1.1387106245543392</v>
       </c>
-      <c r="E15" s="4" t="e">
+      <c r="E15" s="4">
         <f>D12/E12</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F15" s="4" t="e">
+        <v>0.99588546126694377</v>
+      </c>
+      <c r="F15" s="4">
         <f>D12/F12</f>
-        <v>#DIV/0!</v>
+        <v>1.1061825774272125</v>
       </c>
       <c r="G15" s="4" t="e">
         <f>F12/G12</f>
@@ -1905,13 +2024,13 @@
         <f>B12/D12</f>
         <v>1.1622624889895559</v>
       </c>
-      <c r="E16" s="4" t="e">
+      <c r="E16" s="4">
         <f>B12/E12</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F16" s="4" t="e">
+        <v>1.1574803149606299</v>
+      </c>
+      <c r="F16" s="4">
         <f>B12/F12</f>
-        <v>#DIV/0!</v>
+        <v>1.2856745157174341</v>
       </c>
       <c r="G16" s="4" t="e">
         <f>B12/G12</f>
@@ -1921,13 +2040,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B15:G16">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1938,15 +2057,416 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1211</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="4" t="e">
+        <f>AVERAGE(B2:B11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C12" s="4" t="e">
+        <f t="shared" ref="C12:G12" si="0">AVERAGE(C2:C11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D12" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E12" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F12" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G12" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H12" s="4" t="e">
+        <f t="shared" ref="H12:K12" si="1">AVERAGE(H2:H11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I12" s="4" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J12" s="4" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K12" s="4" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="4" t="e">
+        <f>_xlfn.VAR.S(B2:B11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C13" s="4" t="e">
+        <f t="shared" ref="C13:G13" si="2">_xlfn.VAR.S(C2:C11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D13" s="4" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E13" s="4" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F13" s="4" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G13" s="4" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H13" s="4" t="e">
+        <f t="shared" ref="H13:K13" si="3">_xlfn.VAR.S(H2:H11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I13" s="4" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J13" s="4" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K13" s="4" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="30">
+      <c r="A14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4" t="e">
+        <f>1-_xlfn.T.TEST(B2:B11,C2:C11,2,3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D14" s="4" t="e">
+        <f>1-_xlfn.T.TEST(C2:C11,D2:D11,2,3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E14" s="4" t="e">
+        <f>1-_xlfn.T.TEST(D2:D11,E2:E11,2,3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F14" s="4" t="e">
+        <f>1-_xlfn.T.TEST(D2:D11,F2:F11,2,3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G14" s="4" t="e">
+        <f>1-_xlfn.T.TEST(F2:F11,G2:G11,2,3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H14" s="4" t="e">
+        <f t="shared" ref="H14:K14" si="4">1-_xlfn.T.TEST(G2:G11,H2:H11,2,3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I14" s="4" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J14" s="4" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K14" s="4" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="30">
+      <c r="A15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4" t="e">
+        <f>B12/C12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D15" s="4" t="e">
+        <f>C12/D12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E15" s="4" t="e">
+        <f>D12/E12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F15" s="4" t="e">
+        <f>D12/F12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G15" s="4" t="e">
+        <f>F12/G12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H15" s="4" t="e">
+        <f t="shared" ref="H15:K15" si="5">G12/H12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I15" s="4" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J15" s="4" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K15" s="4" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="30">
+      <c r="A16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4" t="e">
+        <f>B12/C12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D16" s="4" t="e">
+        <f>B12/D12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E16" s="4" t="e">
+        <f>B12/E12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F16" s="4" t="e">
+        <f>B12/F12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G16" s="4" t="e">
+        <f>B12/G12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H16" s="4" t="e">
+        <f t="shared" ref="H16:K16" si="6">C12/H12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I16" s="4" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J16" s="4" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K16" s="4" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="B15:K16">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update issue 208 SASL:   Update performance document.
</commit_message>
<xml_diff>
--- a/doc/contents/materials/Performance.xlsx
+++ b/doc/contents/materials/Performance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="20120705" sheetId="1" r:id="rId1"/>
@@ -133,61 +133,7 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -707,11 +653,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="87004672"/>
-        <c:axId val="71669376"/>
+        <c:axId val="145631232"/>
+        <c:axId val="82810496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="87004672"/>
+        <c:axId val="145631232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -720,7 +666,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71669376"/>
+        <c:crossAx val="82810496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -728,7 +674,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71669376"/>
+        <c:axId val="82810496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -739,7 +685,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87004672"/>
+        <c:crossAx val="145631232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1628,13 +1574,13 @@
   <dataConsolidate/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B15:G16">
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1648,8 +1594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection sqref="A1:G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1683,7 +1629,9 @@
       <c r="F1" s="2">
         <v>1211</v>
       </c>
-      <c r="G1" s="2"/>
+      <c r="G1" s="2">
+        <v>1214</v>
+      </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="4">
@@ -1704,7 +1652,9 @@
       <c r="F2" s="4">
         <v>4321</v>
       </c>
-      <c r="G2" s="4"/>
+      <c r="G2" s="4">
+        <v>3206</v>
+      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="4">
@@ -1725,7 +1675,9 @@
       <c r="F3" s="4">
         <v>4334</v>
       </c>
-      <c r="G3" s="4"/>
+      <c r="G3" s="4">
+        <v>3223</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="4">
@@ -1746,7 +1698,9 @@
       <c r="F4" s="4">
         <v>4326</v>
       </c>
-      <c r="G4" s="4"/>
+      <c r="G4" s="4">
+        <v>3238</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="4">
@@ -1767,7 +1721,9 @@
       <c r="F5" s="4">
         <v>4306</v>
       </c>
-      <c r="G5" s="4"/>
+      <c r="G5" s="4">
+        <v>3245</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="4">
@@ -1788,7 +1744,9 @@
       <c r="F6" s="4">
         <v>4295</v>
       </c>
-      <c r="G6" s="4"/>
+      <c r="G6" s="4">
+        <v>3314</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="4">
@@ -1809,7 +1767,9 @@
       <c r="F7" s="4">
         <v>4321</v>
       </c>
-      <c r="G7" s="4"/>
+      <c r="G7" s="4">
+        <v>3248</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4">
@@ -1830,7 +1790,9 @@
       <c r="F8" s="4">
         <v>4314</v>
       </c>
-      <c r="G8" s="4"/>
+      <c r="G8" s="4">
+        <v>3256</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="4">
@@ -1851,7 +1813,9 @@
       <c r="F9" s="4">
         <v>4297</v>
       </c>
-      <c r="G9" s="4"/>
+      <c r="G9" s="4">
+        <v>3226</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="4">
@@ -1872,7 +1836,9 @@
       <c r="F10" s="4">
         <v>4296</v>
       </c>
-      <c r="G10" s="4"/>
+      <c r="G10" s="4">
+        <v>3217</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4">
@@ -1893,7 +1859,9 @@
       <c r="F11" s="4">
         <v>4295</v>
       </c>
-      <c r="G11" s="4"/>
+      <c r="G11" s="4">
+        <v>3223</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="4" t="s">
@@ -1919,9 +1887,9 @@
         <f t="shared" si="0"/>
         <v>4310.5</v>
       </c>
-      <c r="G12" s="4" t="e">
+      <c r="G12" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>3239.6</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1948,9 +1916,9 @@
         <f t="shared" si="1"/>
         <v>213.16666666666666</v>
       </c>
-      <c r="G13" s="4" t="e">
+      <c r="G13" s="4">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>920.26666666666665</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1976,9 +1944,9 @@
         <f>1-_xlfn.T.TEST(D2:D11,F2:F11,2,3)</f>
         <v>1</v>
       </c>
-      <c r="G14" s="4" t="e">
+      <c r="G14" s="4">
         <f>1-_xlfn.T.TEST(F2:F11,G2:G11,2,3)</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -2004,9 +1972,9 @@
         <f>D12/F12</f>
         <v>1.1061825774272125</v>
       </c>
-      <c r="G15" s="4" t="e">
+      <c r="G15" s="4">
         <f>F12/G12</f>
-        <v>#DIV/0!</v>
+        <v>1.3305655019138165</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -2032,21 +2000,21 @@
         <f>B12/F12</f>
         <v>1.2856745157174341</v>
       </c>
-      <c r="G16" s="4" t="e">
+      <c r="G16" s="4">
         <f>B12/G12</f>
-        <v>#DIV/0!</v>
+        <v>1.7106741573033708</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B15:G16">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2059,8 +2027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2072,7 +2040,9 @@
       <c r="B1" s="2">
         <v>1211</v>
       </c>
-      <c r="C1" s="2"/>
+      <c r="C1" s="2">
+        <v>1214</v>
+      </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -2086,8 +2056,12 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="B2" s="4">
+        <v>366</v>
+      </c>
+      <c r="C2" s="4">
+        <v>266</v>
+      </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -2101,8 +2075,12 @@
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="B3" s="4">
+        <v>370</v>
+      </c>
+      <c r="C3" s="4">
+        <v>267</v>
+      </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -2116,8 +2094,12 @@
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="B4" s="4">
+        <v>369</v>
+      </c>
+      <c r="C4" s="4">
+        <v>265</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -2131,8 +2113,12 @@
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="B5" s="4">
+        <v>368</v>
+      </c>
+      <c r="C5" s="4">
+        <v>272</v>
+      </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -2146,8 +2132,12 @@
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="B6" s="4">
+        <v>371</v>
+      </c>
+      <c r="C6" s="4">
+        <v>263</v>
+      </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -2161,8 +2151,12 @@
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="B7" s="4">
+        <v>369</v>
+      </c>
+      <c r="C7" s="4">
+        <v>266</v>
+      </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -2176,8 +2170,12 @@
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="B8" s="4">
+        <v>368</v>
+      </c>
+      <c r="C8" s="4">
+        <v>265</v>
+      </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -2191,8 +2189,12 @@
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="B9" s="4">
+        <v>368</v>
+      </c>
+      <c r="C9" s="4">
+        <v>265</v>
+      </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -2206,8 +2208,12 @@
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
+      <c r="B10" s="4">
+        <v>369</v>
+      </c>
+      <c r="C10" s="4">
+        <v>262</v>
+      </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -2221,8 +2227,12 @@
       <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="B11" s="4">
+        <v>368</v>
+      </c>
+      <c r="C11" s="4">
+        <v>262</v>
+      </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -2236,13 +2246,13 @@
       <c r="A12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="4" t="e">
+      <c r="B12" s="4">
         <f>AVERAGE(B2:B11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C12" s="4" t="e">
+        <v>368.6</v>
+      </c>
+      <c r="C12" s="4">
         <f t="shared" ref="C12:G12" si="0">AVERAGE(C2:C11)</f>
-        <v>#DIV/0!</v>
+        <v>265.3</v>
       </c>
       <c r="D12" s="4" t="e">
         <f t="shared" si="0"/>
@@ -2281,13 +2291,13 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="4" t="e">
+      <c r="B13" s="4">
         <f>_xlfn.VAR.S(B2:B11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C13" s="4" t="e">
+        <v>1.8222222222222224</v>
+      </c>
+      <c r="C13" s="4">
         <f t="shared" ref="C13:G13" si="2">_xlfn.VAR.S(C2:C11)</f>
-        <v>#DIV/0!</v>
+        <v>8.4555555555555539</v>
       </c>
       <c r="D13" s="4" t="e">
         <f t="shared" si="2"/>
@@ -2329,9 +2339,9 @@
       <c r="B14" s="4">
         <v>0</v>
       </c>
-      <c r="C14" s="4" t="e">
+      <c r="C14" s="4">
         <f>1-_xlfn.T.TEST(B2:B11,C2:C11,2,3)</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="D14" s="4" t="e">
         <f>1-_xlfn.T.TEST(C2:C11,D2:D11,2,3)</f>
@@ -2373,9 +2383,9 @@
       <c r="B15" s="4">
         <v>1</v>
       </c>
-      <c r="C15" s="4" t="e">
+      <c r="C15" s="4">
         <f>B12/C12</f>
-        <v>#DIV/0!</v>
+        <v>1.3893705239351677</v>
       </c>
       <c r="D15" s="4" t="e">
         <f>C12/D12</f>
@@ -2417,9 +2427,9 @@
       <c r="B16" s="4">
         <v>1</v>
       </c>
-      <c r="C16" s="4" t="e">
+      <c r="C16" s="4">
         <f>B12/C12</f>
-        <v>#DIV/0!</v>
+        <v>1.3893705239351677</v>
       </c>
       <c r="D16" s="4" t="e">
         <f>B12/D12</f>
@@ -2457,13 +2467,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B15:K16">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>